<commit_message>
Met à jour les résultats
</commit_message>
<xml_diff>
--- a/Docs/Résultats/Résultats_04_11_15.xlsx
+++ b/Docs/Résultats/Résultats_04_11_15.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
   <si>
     <t>Titre</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>Non prise en compte du dernier onset attendu dans l'évaluation</t>
+  </si>
+  <si>
+    <t>Conséquence =&gt; l'onset est en retard par rapport à la réalité =&gt; la note est mal analysée en ton</t>
   </si>
 </sst>
 </file>
@@ -611,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,19 +1030,19 @@
         <v>0.95</v>
       </c>
       <c r="H18" s="4">
-        <v>0.57140000000000002</v>
+        <v>0.55549999999999999</v>
       </c>
       <c r="I18" s="4">
+        <v>0.44440000000000002</v>
+      </c>
+      <c r="J18" s="21">
         <v>0.35709999999999997</v>
       </c>
-      <c r="J18" s="21">
-        <v>0.34279999999999999</v>
-      </c>
       <c r="K18" s="26">
-        <v>0.57140000000000002</v>
+        <v>0.44440000000000002</v>
       </c>
       <c r="L18" s="22">
-        <v>0.78569999999999995</v>
+        <v>0.94440000000000002</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -1115,7 +1118,7 @@
         <v>1</v>
       </c>
       <c r="J20" s="14">
-        <v>0.96</v>
+        <v>0.96599999999999997</v>
       </c>
       <c r="K20" s="6">
         <v>0</v>
@@ -1191,10 +1194,10 @@
         <v>0.89130434782608703</v>
       </c>
       <c r="H22" s="6">
-        <v>0.84199999999999997</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="I22" s="6">
-        <v>0.71052000000000004</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="J22" s="14">
         <v>0.5</v>
@@ -1203,7 +1206,7 @@
         <v>7.8899999999999998E-2</v>
       </c>
       <c r="L22" s="7">
-        <v>0.57899999999999996</v>
+        <v>0.89129999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1232,19 +1235,19 @@
         <v>0.88888888888888884</v>
       </c>
       <c r="H23" s="11">
-        <v>0.73839999999999995</v>
+        <v>0.78869999999999996</v>
       </c>
       <c r="I23" s="10">
-        <v>0.61529999999999996</v>
+        <v>0.57740000000000002</v>
       </c>
       <c r="J23" s="20">
         <v>0.59670000000000001</v>
       </c>
       <c r="K23" s="11">
-        <v>7.6899999999999996E-2</v>
+        <v>0.11260000000000001</v>
       </c>
       <c r="L23" s="12">
-        <v>0.76919999999999999</v>
+        <v>0.76049999999999995</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -1265,23 +1268,23 @@
       </c>
       <c r="H24" s="19">
         <f t="shared" ref="H24" si="11">AVERAGE(H18:H23)</f>
-        <v>0.69196666666666662</v>
+        <v>0.69486666666666663</v>
       </c>
       <c r="I24" s="19">
         <f t="shared" ref="I24" si="12">AVERAGE(I18:I23)</f>
-        <v>0.61381999999999992</v>
+        <v>0.61613333333333331</v>
       </c>
       <c r="J24" s="19">
         <f t="shared" ref="J24" si="13">AVERAGE(J18:J23)</f>
-        <v>0.39991666666666664</v>
+        <v>0.40329999999999999</v>
       </c>
       <c r="K24" s="19">
         <f t="shared" ref="K24" si="14">AVERAGE(K18:K23)</f>
-        <v>0.4545333333333334</v>
+        <v>0.43931666666666663</v>
       </c>
       <c r="L24" s="19">
         <f t="shared" ref="L24" si="15">AVERAGE(L18:L23)</f>
-        <v>0.85564999999999991</v>
+        <v>0.93269999999999997</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -1332,22 +1335,25 @@
         <v>8.8888888888888893</v>
       </c>
     </row>
-    <row r="34" spans="3:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="3:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="H35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>26</v>
       </c>

</xml_diff>